<commit_message>
Noise Score * 0.1, general score adjust weight, clarity using minus sign
</commit_message>
<xml_diff>
--- a/scores.xlsx
+++ b/scores.xlsx
@@ -525,7 +525,7 @@
         <v>4.715941985645933</v>
       </c>
       <c r="C2" t="n">
-        <v>42.22223211119788</v>
+        <v>4.222223211119789</v>
       </c>
       <c r="D2" t="n">
         <v>16.55774271987239</v>
@@ -534,13 +534,13 @@
         <v>24.00812943631453</v>
       </c>
       <c r="F2" t="n">
-        <v>8.178140958007422</v>
+        <v>2.559317730011622</v>
       </c>
       <c r="G2" t="n">
         <v>3.17873096110801</v>
       </c>
       <c r="H2" t="n">
-        <v>46.25373463539849</v>
+        <v>4.625373463539849</v>
       </c>
       <c r="I2" t="n">
         <v>18.1387193222021</v>
@@ -549,22 +549,22 @@
         <v>36.27592441028044</v>
       </c>
       <c r="K2" t="n">
-        <v>11.1566401084279</v>
+        <v>4.596231881963304</v>
       </c>
       <c r="L2" t="n">
-        <v>1.366148325358852</v>
+        <v>17.28446471291866</v>
       </c>
       <c r="M2" t="n">
-        <v>41.03703920562463</v>
+        <v>4.991295985400049</v>
       </c>
       <c r="N2" t="n">
-        <v>16.09295655122535</v>
+        <v>19.57371478280446</v>
       </c>
       <c r="O2" t="n">
-        <v>23.57897093021315</v>
+        <v>24.12717311370862</v>
       </c>
       <c r="P2" t="n">
-        <v>6.735037998890091</v>
+        <v>-2.083714412855725</v>
       </c>
     </row>
     <row r="3">
@@ -577,7 +577,7 @@
         <v>2.036041728158205</v>
       </c>
       <c r="C3" t="n">
-        <v>36.03150636177188</v>
+        <v>3.603150636177189</v>
       </c>
       <c r="D3" t="n">
         <v>14.1300024948125</v>
@@ -586,13 +586,13 @@
         <v>20.61784267712213</v>
       </c>
       <c r="F3" t="n">
-        <v>6.222619357185232</v>
+        <v>2.992422884558274</v>
       </c>
       <c r="G3" t="n">
         <v>1.554924312067169</v>
       </c>
       <c r="H3" t="n">
-        <v>52.98765881831494</v>
+        <v>5.298765881831494</v>
       </c>
       <c r="I3" t="n">
         <v>20.77947442072099</v>
@@ -601,22 +601,22 @@
         <v>25.73683853237733</v>
       </c>
       <c r="K3" t="n">
-        <v>7.20015028685277</v>
+        <v>4.517979248005615</v>
       </c>
       <c r="L3" t="n">
-        <v>1.009339027449823</v>
+        <v>6.225969414108619</v>
       </c>
       <c r="M3" t="n">
-        <v>35.19276446731414</v>
+        <v>3.969817732951864</v>
       </c>
       <c r="N3" t="n">
-        <v>13.80108410482908</v>
+        <v>15.56790661812184</v>
       </c>
       <c r="O3" t="n">
-        <v>20.53434613615186</v>
+        <v>20.41216723425281</v>
       </c>
       <c r="P3" t="n">
-        <v>5.804979826059888</v>
+        <v>1.473464961520643</v>
       </c>
     </row>
     <row r="4">
@@ -629,7 +629,7 @@
         <v>18.42103913685592</v>
       </c>
       <c r="C4" t="n">
-        <v>64.72339220569529</v>
+        <v>6.47233922056953</v>
       </c>
       <c r="D4" t="n">
         <v>25.38172241090424</v>
@@ -638,13 +638,13 @@
         <v>39.7800072343436</v>
       </c>
       <c r="F4" t="n">
-        <v>17.90642308665677</v>
+        <v>-0.2557722152980224</v>
       </c>
       <c r="G4" t="n">
         <v>0.7160848620296953</v>
       </c>
       <c r="H4" t="n">
-        <v>51.30961586720532</v>
+        <v>5.130961586720532</v>
       </c>
       <c r="I4" t="n">
         <v>20.12141798713934</v>
@@ -653,22 +653,22 @@
         <v>33.01705743355363</v>
       </c>
       <c r="K4" t="n">
-        <v>9.084873185585304</v>
+        <v>5.500266919955192</v>
       </c>
       <c r="L4" t="n">
-        <v>3.400313833278635</v>
+        <v>66.21822899573351</v>
       </c>
       <c r="M4" t="n">
-        <v>57.867346775904</v>
+        <v>9.497148630804267</v>
       </c>
       <c r="N4" t="n">
-        <v>22.69307716702118</v>
+        <v>37.24370443203261</v>
       </c>
       <c r="O4" t="n">
-        <v>37.933370245896</v>
+        <v>28.16507224873779</v>
       </c>
       <c r="P4" t="n">
-        <v>11.49201736289409</v>
+        <v>-19.07118807625439</v>
       </c>
     </row>
     <row r="5">
@@ -681,7 +681,7 @@
         <v>3.684851942663146</v>
       </c>
       <c r="C5" t="n">
-        <v>61.46790816742585</v>
+        <v>6.146790816742586</v>
       </c>
       <c r="D5" t="n">
         <v>24.10506202644151</v>
@@ -690,13 +690,13 @@
         <v>24.32825177947639</v>
       </c>
       <c r="F5" t="n">
-        <v>7.446637899453892</v>
+        <v>3.935859561147907</v>
       </c>
       <c r="G5" t="n">
         <v>1.914196279270304</v>
       </c>
       <c r="H5" t="n">
-        <v>75.80557933448844</v>
+        <v>7.580557933448844</v>
       </c>
       <c r="I5" t="n">
         <v>29.72768217147128</v>
@@ -705,22 +705,22 @@
         <v>49.22550411177843</v>
       </c>
       <c r="K5" t="n">
-        <v>13.89830824608706</v>
+        <v>7.828240953729322</v>
       </c>
       <c r="L5" t="n">
-        <v>1.347104866088269</v>
+        <v>13.26006412674463</v>
       </c>
       <c r="M5" t="n">
-        <v>60.25095583558616</v>
+        <v>6.52599831047601</v>
       </c>
       <c r="N5" t="n">
-        <v>23.62782581787693</v>
+        <v>25.59214867785863</v>
       </c>
       <c r="O5" t="n">
-        <v>23.70734573984063</v>
+        <v>24.36611026990594</v>
       </c>
       <c r="P5" t="n">
-        <v>6.351515248404264</v>
+        <v>0.2932156187216668</v>
       </c>
     </row>
     <row r="6">
@@ -733,7 +733,7 @@
         <v>2.71779154247392</v>
       </c>
       <c r="C6" t="n">
-        <v>65.18309386226511</v>
+        <v>6.518309386226512</v>
       </c>
       <c r="D6" t="n">
         <v>25.56199709051231</v>
@@ -742,13 +742,13 @@
         <v>19.9398357625764</v>
       </c>
       <c r="F6" t="n">
-        <v>5.663157377638437</v>
+        <v>4.06377356150258</v>
       </c>
       <c r="G6" t="n">
         <v>2.065419636754223</v>
       </c>
       <c r="H6" t="n">
-        <v>42.70193039325233</v>
+        <v>4.270193039325234</v>
       </c>
       <c r="I6" t="n">
         <v>16.74585533248155</v>
@@ -757,22 +757,22 @@
         <v>22.35601667923642</v>
       </c>
       <c r="K6" t="n">
-        <v>6.611950885643691</v>
+        <v>3.477546967920692</v>
       </c>
       <c r="L6" t="n">
-        <v>0.9009864008941878</v>
+        <v>10.03842026825633</v>
       </c>
       <c r="M6" t="n">
-        <v>64.91296563128455</v>
+        <v>6.777379886930184</v>
       </c>
       <c r="N6" t="n">
-        <v>25.45606495344492</v>
+        <v>26.57795115592092</v>
       </c>
       <c r="O6" t="n">
-        <v>19.83575937026487</v>
+        <v>19.77648636999793</v>
       </c>
       <c r="P6" t="n">
-        <v>4.911038798997665</v>
+        <v>1.244656794802388</v>
       </c>
     </row>
     <row r="7">
@@ -785,7 +785,7 @@
         <v>3.779955368447708</v>
       </c>
       <c r="C7" t="n">
-        <v>65.56708149125991</v>
+        <v>6.556708149125992</v>
       </c>
       <c r="D7" t="n">
         <v>25.71258097696467</v>
@@ -794,13 +794,13 @@
         <v>33.19422744025417</v>
       </c>
       <c r="F7" t="n">
-        <v>10.05605842572228</v>
+        <v>4.98294434730147</v>
       </c>
       <c r="G7" t="n">
         <v>0.9272868098872874</v>
       </c>
       <c r="H7" t="n">
-        <v>67.55608589823039</v>
+        <v>6.75560858982304</v>
       </c>
       <c r="I7" t="n">
         <v>26.49258270518839</v>
@@ -809,22 +809,22 @@
         <v>32.10661106155546</v>
       </c>
       <c r="K7" t="n">
-        <v>8.54580599363619</v>
+        <v>6.111580346291397</v>
       </c>
       <c r="L7" t="n">
-        <v>1.737731071157255</v>
+        <v>12.11808844011142</v>
       </c>
       <c r="M7" t="n">
-        <v>64.63440191861908</v>
+        <v>6.963023438158046</v>
       </c>
       <c r="N7" t="n">
-        <v>25.3468242818114</v>
+        <v>27.30597826817089</v>
       </c>
       <c r="O7" t="n">
-        <v>33.00204401635291</v>
+        <v>33.21571584114716</v>
       </c>
       <c r="P7" t="n">
-        <v>9.201630297869148</v>
+        <v>1.846624830256911</v>
       </c>
     </row>
     <row r="8">
@@ -837,7 +837,7 @@
         <v>1.447986270433037</v>
       </c>
       <c r="C8" t="n">
-        <v>26.6072378715509</v>
+        <v>2.66072378715509</v>
       </c>
       <c r="D8" t="n">
         <v>10.43421011871853</v>
@@ -846,13 +846,13 @@
         <v>32.12825861709734</v>
       </c>
       <c r="F8" t="n">
-        <v>9.643790329891035</v>
+        <v>3.922256241133697</v>
       </c>
       <c r="G8" t="n">
         <v>0.3822582273517379</v>
       </c>
       <c r="H8" t="n">
-        <v>26.64165717176652</v>
+        <v>2.664165717176652</v>
       </c>
       <c r="I8" t="n">
         <v>10.4477086948104</v>
@@ -861,22 +861,22 @@
         <v>32.08365512679532</v>
       </c>
       <c r="K8" t="n">
-        <v>9.203375850764719</v>
+        <v>4.345754245547921</v>
       </c>
       <c r="L8" t="n">
-        <v>0.4441425293948953</v>
+        <v>5.413915973616289</v>
       </c>
       <c r="M8" t="n">
-        <v>26.38251844412708</v>
+        <v>2.816777870994172</v>
       </c>
       <c r="N8" t="n">
-        <v>10.34608566436356</v>
+        <v>11.04618637067342</v>
       </c>
       <c r="O8" t="n">
-        <v>31.90160749070559</v>
+        <v>32.21762696552921</v>
       </c>
       <c r="P8" t="n">
-        <v>9.179104547429638</v>
+        <v>2.420400219942837</v>
       </c>
     </row>
     <row r="9">
@@ -889,7 +889,7 @@
         <v>7.702746652572234</v>
       </c>
       <c r="C9" t="n">
-        <v>44.15755032557821</v>
+        <v>4.415755032557821</v>
       </c>
       <c r="D9" t="n">
         <v>17.31668640218753</v>
@@ -898,13 +898,13 @@
         <v>34.68324433125234</v>
       </c>
       <c r="F9" t="n">
-        <v>12.53365420828428</v>
+        <v>2.5258365427665</v>
       </c>
       <c r="G9" t="n">
         <v>0.6186927752210684</v>
       </c>
       <c r="H9" t="n">
-        <v>36.63880465358451</v>
+        <v>3.663880465358452</v>
       </c>
       <c r="I9" t="n">
         <v>14.36815855339739</v>
@@ -913,22 +913,22 @@
         <v>20.70763140711556</v>
       </c>
       <c r="K9" t="n">
-        <v>5.669517777544121</v>
+        <v>3.597753601695072</v>
       </c>
       <c r="L9" t="n">
-        <v>2.457288583509514</v>
+        <v>25.94161733615222</v>
       </c>
       <c r="M9" t="n">
-        <v>40.75908435201401</v>
+        <v>6.245329638807759</v>
       </c>
       <c r="N9" t="n">
-        <v>15.98395464784863</v>
+        <v>24.49149171334361</v>
       </c>
       <c r="O9" t="n">
-        <v>34.37733834447735</v>
+        <v>34.120233169054</v>
       </c>
       <c r="P9" t="n">
-        <v>10.41699943111534</v>
+        <v>-3.939924166529095</v>
       </c>
     </row>
     <row r="10">
@@ -941,7 +941,7 @@
         <v>4.512147956510349</v>
       </c>
       <c r="C10" t="n">
-        <v>51.16708529804799</v>
+        <v>5.1167085298048</v>
       </c>
       <c r="D10" t="n">
         <v>20.06552364629333</v>
@@ -950,13 +950,13 @@
         <v>37.2489788626585</v>
       </c>
       <c r="F10" t="n">
-        <v>11.87594904085556</v>
+        <v>4.398130873978936</v>
       </c>
       <c r="G10" t="n">
         <v>4.142267114882431</v>
       </c>
       <c r="H10" t="n">
-        <v>64.99956041147649</v>
+        <v>6.49995604114765</v>
       </c>
       <c r="I10" t="n">
         <v>25.49002347324639</v>
@@ -965,22 +965,22 @@
         <v>29.99256628928473</v>
       </c>
       <c r="K10" t="n">
-        <v>9.252725386240019</v>
+        <v>4.490367665280484</v>
       </c>
       <c r="L10" t="n">
-        <v>1.082997118155619</v>
+        <v>14.87813073094053</v>
       </c>
       <c r="M10" t="n">
-        <v>50.51310236631329</v>
+        <v>5.600666246139735</v>
       </c>
       <c r="N10" t="n">
-        <v>19.80905975149541</v>
+        <v>21.96339552362443</v>
       </c>
       <c r="O10" t="n">
-        <v>34.08780499832672</v>
+        <v>36.26854107813476</v>
       </c>
       <c r="P10" t="n">
-        <v>9.570042060428014</v>
+        <v>0.3880810463202282</v>
       </c>
     </row>
     <row r="11">
@@ -993,7 +993,7 @@
         <v>3.254099219540396</v>
       </c>
       <c r="C11" t="n">
-        <v>65.36881959765681</v>
+        <v>6.536881959765681</v>
       </c>
       <c r="D11" t="n">
         <v>25.63483121476738</v>
@@ -1002,13 +1002,13 @@
         <v>28.69060294051243</v>
       </c>
       <c r="F11" t="n">
-        <v>8.498904853157683</v>
+        <v>4.733322261258856</v>
       </c>
       <c r="G11" t="n">
         <v>0.5750958818698866</v>
       </c>
       <c r="H11" t="n">
-        <v>65.96221032500618</v>
+        <v>6.596221032500619</v>
       </c>
       <c r="I11" t="n">
         <v>25.86753346078674</v>
@@ -1017,22 +1017,22 @@
         <v>20.04039749552189</v>
       </c>
       <c r="K11" t="n">
-        <v>4.81944326106125</v>
+        <v>4.968641779211397</v>
       </c>
       <c r="L11" t="n">
-        <v>1.398666714843185</v>
+        <v>10.52265320132967</v>
       </c>
       <c r="M11" t="n">
-        <v>64.3970570169823</v>
+        <v>6.925087483223781</v>
       </c>
       <c r="N11" t="n">
-        <v>25.25374784979698</v>
+        <v>27.15720405473038</v>
       </c>
       <c r="O11" t="n">
-        <v>28.54029601833661</v>
+        <v>27.49027811796294</v>
       </c>
       <c r="P11" t="n">
-        <v>7.732599359699424</v>
+        <v>1.893881097243367</v>
       </c>
     </row>
     <row r="12">
@@ -1045,7 +1045,7 @@
         <v>5.837056497577658</v>
       </c>
       <c r="C12" t="n">
-        <v>58.28319888439398</v>
+        <v>5.828319888439398</v>
       </c>
       <c r="D12" t="n">
         <v>22.85615642525254</v>
@@ -1054,13 +1054,13 @@
         <v>32.35556476706021</v>
       </c>
       <c r="F12" t="n">
-        <v>10.78440342576024</v>
+        <v>3.723469196193645</v>
       </c>
       <c r="G12" t="n">
         <v>1.1819081645297</v>
       </c>
       <c r="H12" t="n">
-        <v>66.06916958428691</v>
+        <v>6.606916958428691</v>
       </c>
       <c r="I12" t="n">
         <v>25.90947812867401</v>
@@ -1069,22 +1069,22 @@
         <v>28.96321554517722</v>
       </c>
       <c r="K12" t="n">
-        <v>7.736706596671159</v>
+        <v>5.623378826912037</v>
       </c>
       <c r="L12" t="n">
-        <v>2.227755414648048</v>
+        <v>17.08750890567113</v>
       </c>
       <c r="M12" t="n">
-        <v>56.36169645466154</v>
+        <v>6.703110813527243</v>
       </c>
       <c r="N12" t="n">
-        <v>22.10262606065158</v>
+        <v>26.28671813211271</v>
       </c>
       <c r="O12" t="n">
-        <v>31.12070991631914</v>
+        <v>32.68543386540362</v>
       </c>
       <c r="P12" t="n">
-        <v>9.011670707419123</v>
+        <v>-0.3200497933637232</v>
       </c>
     </row>
     <row r="13">
@@ -1097,7 +1097,7 @@
         <v>9.773338441985645</v>
       </c>
       <c r="C13" t="n">
-        <v>46.0627233099522</v>
+        <v>4.60627233099522</v>
       </c>
       <c r="D13" t="n">
         <v>18.06381213521527</v>
@@ -1106,13 +1106,13 @@
         <v>37.96894048800728</v>
       </c>
       <c r="F13" t="n">
-        <v>14.30650761924428</v>
+        <v>2.118439399750958</v>
       </c>
       <c r="G13" t="n">
         <v>0.6224575697008706</v>
       </c>
       <c r="H13" t="n">
-        <v>61.99419495745683</v>
+        <v>6.199419495745683</v>
       </c>
       <c r="I13" t="n">
         <v>24.31144900292425</v>
@@ -1121,22 +1121,22 @@
         <v>23.09843530915621</v>
       </c>
       <c r="K13" t="n">
-        <v>5.841383925466378</v>
+        <v>5.063324454896417</v>
       </c>
       <c r="L13" t="n">
-        <v>2.238450396232057</v>
+        <v>24.56446153558612</v>
       </c>
       <c r="M13" t="n">
-        <v>43.24324738904041</v>
+        <v>5.729196073446793</v>
       </c>
       <c r="N13" t="n">
-        <v>16.95813685440777</v>
+        <v>22.46744359205555</v>
       </c>
       <c r="O13" t="n">
-        <v>25.77087513892217</v>
+        <v>34.6814946209151</v>
       </c>
       <c r="P13" t="n">
-        <v>7.693945332146987</v>
+        <v>-3.582905255765869</v>
       </c>
     </row>
     <row r="14">
@@ -1149,7 +1149,7 @@
         <v>4.974390825198292</v>
       </c>
       <c r="C14" t="n">
-        <v>41.21325032780346</v>
+        <v>4.121325032780346</v>
       </c>
       <c r="D14" t="n">
         <v>16.16206127270449</v>
@@ -1158,13 +1158,13 @@
         <v>27.66504941777041</v>
       </c>
       <c r="F14" t="n">
-        <v>9.400358377170992</v>
+        <v>2.772763356404518</v>
       </c>
       <c r="G14" t="n">
         <v>1.189381202450474</v>
       </c>
       <c r="H14" t="n">
-        <v>41.53789391957205</v>
+        <v>4.153789391957205</v>
       </c>
       <c r="I14" t="n">
         <v>16.28937016453806</v>
@@ -1173,22 +1173,22 @@
         <v>27.5475491563857</v>
       </c>
       <c r="K14" t="n">
-        <v>7.844101868846305</v>
+        <v>4.29073964997883</v>
       </c>
       <c r="L14" t="n">
-        <v>1.665155010677242</v>
+        <v>17.42986386516169</v>
       </c>
       <c r="M14" t="n">
-        <v>39.19350698318627</v>
+        <v>5.273489849649542</v>
       </c>
       <c r="N14" t="n">
-        <v>15.37000273850442</v>
+        <v>20.68035584584088</v>
       </c>
       <c r="O14" t="n">
-        <v>27.29789635250295</v>
+        <v>27.88213341330816</v>
       </c>
       <c r="P14" t="n">
-        <v>8.010080759404037</v>
+        <v>-1.629707990460545</v>
       </c>
     </row>
     <row r="15">
@@ -1201,7 +1201,7 @@
         <v>6.37260101010101</v>
       </c>
       <c r="C15" t="n">
-        <v>52.47114828446551</v>
+        <v>5.247114828446552</v>
       </c>
       <c r="D15" t="n">
         <v>20.57692089586883</v>
@@ -1210,13 +1210,13 @@
         <v>29.35888224747742</v>
       </c>
       <c r="F15" t="n">
-        <v>10.22497442901084</v>
+        <v>2.928097551347136</v>
       </c>
       <c r="G15" t="n">
         <v>0.8682371538949296</v>
       </c>
       <c r="H15" t="n">
-        <v>66.41397232977872</v>
+        <v>6.641397232977872</v>
       </c>
       <c r="I15" t="n">
         <v>26.04469503128577</v>
@@ -1225,22 +1225,22 @@
         <v>20.47413757137727</v>
       </c>
       <c r="K15" t="n">
-        <v>5.057077906250434</v>
+        <v>4.916638731943547</v>
       </c>
       <c r="L15" t="n">
-        <v>1.89518837018837</v>
+        <v>21.26021532896533</v>
       </c>
       <c r="M15" t="n">
-        <v>51.1119871117759</v>
+        <v>6.291667134464745</v>
       </c>
       <c r="N15" t="n">
-        <v>20.04391651442192</v>
+        <v>24.67319773979009</v>
       </c>
       <c r="O15" t="n">
-        <v>25.84874014457802</v>
+        <v>29.00189139299194</v>
       </c>
       <c r="P15" t="n">
-        <v>7.410281983155547</v>
+        <v>-2.556757584668345</v>
       </c>
     </row>
     <row r="16">
@@ -1253,7 +1253,7 @@
         <v>6.557349793064079</v>
       </c>
       <c r="C16" t="n">
-        <v>71.80938274560448</v>
+        <v>7.180938274560448</v>
       </c>
       <c r="D16" t="n">
         <v>28.16055001301847</v>
@@ -1262,13 +1262,13 @@
         <v>49.45750816275599</v>
       </c>
       <c r="F16" t="n">
-        <v>15.91136409409567</v>
+        <v>5.800639419285525</v>
       </c>
       <c r="G16" t="n">
         <v>5.232141182695592</v>
       </c>
       <c r="H16" t="n">
-        <v>67.06349672525378</v>
+        <v>6.706349672525379</v>
       </c>
       <c r="I16" t="n">
         <v>26.29941105022611</v>
@@ -1277,22 +1277,22 @@
         <v>38.40833148548268</v>
       </c>
       <c r="K16" t="n">
-        <v>12.16888845624288</v>
+        <v>4.995953983757638</v>
       </c>
       <c r="L16" t="n">
-        <v>2.424721706864564</v>
+        <v>18.88898423005566</v>
       </c>
       <c r="M16" t="n">
-        <v>70.50451626235278</v>
+        <v>7.732042190561645</v>
       </c>
       <c r="N16" t="n">
-        <v>27.64883018123329</v>
+        <v>30.32174623946256</v>
       </c>
       <c r="O16" t="n">
-        <v>45.69008443724165</v>
+        <v>46.06058367156609</v>
       </c>
       <c r="P16" t="n">
-        <v>13.1562284239297</v>
+        <v>0.7952012658583634</v>
       </c>
     </row>
     <row r="17">
@@ -1305,7 +1305,7 @@
         <v>3.956701308975834</v>
       </c>
       <c r="C17" t="n">
-        <v>64.44960907057917</v>
+        <v>6.444960907057918</v>
       </c>
       <c r="D17" t="n">
         <v>25.27435649826634</v>
@@ -1314,13 +1314,13 @@
         <v>21.25681966221678</v>
       </c>
       <c r="F17" t="n">
-        <v>6.569636814850718</v>
+        <v>3.664384470167237</v>
       </c>
       <c r="G17" t="n">
         <v>2.690897953080754</v>
       </c>
       <c r="H17" t="n">
-        <v>48.59696759510381</v>
+        <v>4.859696759510381</v>
       </c>
       <c r="I17" t="n">
         <v>19.05763574997651</v>
@@ -1329,22 +1329,22 @@
         <v>27.33400426593479</v>
       </c>
       <c r="K17" t="n">
-        <v>8.228390851497659</v>
+        <v>4.010659367503363</v>
       </c>
       <c r="L17" t="n">
-        <v>1.115828178941312</v>
+        <v>14.472166283084</v>
       </c>
       <c r="M17" t="n">
-        <v>63.81907297385261</v>
+        <v>6.87898557916335</v>
       </c>
       <c r="N17" t="n">
-        <v>25.02708744072651</v>
+        <v>26.97641662188543</v>
       </c>
       <c r="O17" t="n">
-        <v>20.65238190328456</v>
+        <v>21.35423951342748</v>
       </c>
       <c r="P17" t="n">
-        <v>5.265556033321936</v>
+        <v>-0.3218549112627729</v>
       </c>
     </row>
   </sheetData>

</xml_diff>